<commit_message>
updated schematic started on relearning stm32f0
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -587,7 +587,7 @@
   <dimension ref="B2:J1330"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +752,9 @@
       <c r="E11" s="9">
         <v>42580</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9">
+        <v>42577</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>45</v>
       </c>

</xml_diff>